<commit_message>
Update stats and script
</commit_message>
<xml_diff>
--- a/report/stats.xlsx
+++ b/report/stats.xlsx
@@ -24,23 +24,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
   <si>
-    <t>Positions</t>
+    <t>Game</t>
   </si>
   <si>
-    <t>Agent Score</t>
+    <t>Game Num</t>
   </si>
   <si>
-    <t>Difference</t>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Difference b/w First</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>bucephalus</t>
+  </si>
+  <si>
+    <t>AgentElman</t>
+  </si>
+  <si>
+    <t>westridge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,205 +377,1000 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>616</v>
+      </c>
+      <c r="D2">
+        <v>1708.04</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2116.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>619</v>
+      </c>
+      <c r="D3">
+        <v>-1573.05</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>3604.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>621</v>
+      </c>
+      <c r="D4">
+        <v>-260.16000000000003</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>2922.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>623</v>
+      </c>
+      <c r="D5">
+        <v>109.1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>3489.51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>626</v>
+      </c>
+      <c r="D6">
+        <v>-960.39</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>3292.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>630</v>
+      </c>
+      <c r="D7">
+        <v>3495.15</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>60.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>633</v>
+      </c>
+      <c r="D8">
+        <v>2840.66</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>2192.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>634</v>
+      </c>
+      <c r="D9">
+        <v>2076.5700000000002</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>721.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>637</v>
+      </c>
+      <c r="D10">
+        <v>-1249.8599999999999</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>4199.8599999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>640</v>
+      </c>
+      <c r="D11">
+        <v>2305.23</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>641</v>
+      </c>
+      <c r="D12">
+        <v>3163.09</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>600.21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>642</v>
+      </c>
+      <c r="D13">
+        <v>-1053.01</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2096.37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>646</v>
+      </c>
+      <c r="D14">
+        <v>3425.59</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>428.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>650</v>
+      </c>
+      <c r="D15">
+        <v>1930</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>1807.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>654</v>
+      </c>
+      <c r="D16">
+        <v>3341.38</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>827.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>655</v>
+      </c>
+      <c r="D17">
+        <v>2331.38</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>490.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>613</v>
+      </c>
+      <c r="D20">
+        <v>2436.66</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1713.78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>615</v>
+      </c>
+      <c r="D21">
+        <v>2367.39</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>1314.37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>616</v>
+      </c>
+      <c r="D22">
+        <v>845.47</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>2978.73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>623</v>
+      </c>
+      <c r="D23">
+        <v>3598.61</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>624</v>
+      </c>
+      <c r="D24">
+        <v>3265.73</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>1171.17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>627</v>
+      </c>
+      <c r="D25">
+        <v>2061.04</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1119.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>629</v>
+      </c>
+      <c r="D26">
+        <v>-1052.32</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>5368.55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>633</v>
+      </c>
+      <c r="D27">
+        <v>3431.66</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1601.27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>636</v>
+      </c>
+      <c r="D28">
+        <v>3858.19</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>640</v>
+      </c>
+      <c r="D29">
+        <v>634.41999999999996</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>1670.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>643</v>
+      </c>
+      <c r="D30">
+        <v>389.21</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>1361.83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>644</v>
+      </c>
+      <c r="D31">
+        <v>3046.4</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>646</v>
+      </c>
+      <c r="D32">
+        <v>3854.19</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>649</v>
+      </c>
+      <c r="D33">
+        <v>2612.69</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>654</v>
+      </c>
+      <c r="D34">
+        <v>4168.42</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>656</v>
+      </c>
+      <c r="D35">
+        <v>2365.04</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>1463.35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>614</v>
+      </c>
+      <c r="D37">
         <v>3640.02</v>
       </c>
-      <c r="E2">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>618</v>
+      </c>
+      <c r="D38">
+        <v>2517.67</v>
+      </c>
+      <c r="E38">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>2517.67</v>
-      </c>
-      <c r="E3">
+      <c r="F38">
         <v>1358.91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>620</v>
+      </c>
+      <c r="D39">
         <v>3108.83</v>
       </c>
-      <c r="E4">
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
         <v>466</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>622</v>
+      </c>
+      <c r="D40">
         <v>3133.48</v>
       </c>
-      <c r="E5">
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
         <v>536.79999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="C6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>626</v>
+      </c>
+      <c r="D41">
         <v>787.68</v>
       </c>
-      <c r="E6">
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
         <v>1544.32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>629</v>
+      </c>
+      <c r="D42">
+        <v>3029.65</v>
+      </c>
+      <c r="E42">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>3029.65</v>
-      </c>
-      <c r="E7">
+      <c r="F42">
         <v>1286.58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>632</v>
+      </c>
+      <c r="D43">
+        <v>3113.59</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>3113.59</v>
-      </c>
-      <c r="E8">
+      <c r="F43">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="C9">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>634</v>
+      </c>
+      <c r="D44">
         <v>1601.57</v>
       </c>
-      <c r="E9">
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
         <v>1196.3699999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="C10">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>635</v>
+      </c>
+      <c r="D45">
         <v>-227.45</v>
       </c>
-      <c r="E10">
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
         <v>2593.3200000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>637</v>
+      </c>
+      <c r="D46">
+        <v>1183.4100000000001</v>
+      </c>
+      <c r="E46">
         <v>3</v>
       </c>
-      <c r="C11">
-        <v>1183.4100000000001</v>
-      </c>
-      <c r="E11">
+      <c r="F46">
         <v>1766.59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="C12">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>642</v>
+      </c>
+      <c r="D47">
         <v>611.42999999999995</v>
       </c>
-      <c r="E12">
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
         <v>431.93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>12</v>
+      </c>
+      <c r="C48">
+        <v>643</v>
+      </c>
+      <c r="D48">
+        <v>674.42</v>
+      </c>
+      <c r="E48">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>674.42</v>
-      </c>
-      <c r="E13">
+      <c r="F48">
         <v>1076.6199999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>647</v>
+      </c>
+      <c r="D49">
+        <v>2451.2199999999998</v>
+      </c>
+      <c r="E49">
         <v>3</v>
       </c>
-      <c r="C14">
-        <v>2451.2199999999998</v>
-      </c>
-      <c r="E14">
+      <c r="F49">
         <v>569.28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="C15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>650</v>
+      </c>
+      <c r="D50">
         <v>3657</v>
       </c>
-      <c r="E15">
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
         <v>80.8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>653</v>
+      </c>
+      <c r="D51">
+        <v>4475.46</v>
+      </c>
+      <c r="E51">
         <v>1</v>
       </c>
-      <c r="C16">
-        <v>4475.46</v>
-      </c>
-      <c r="E16">
+      <c r="F51">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>656</v>
+      </c>
+      <c r="D52">
+        <v>703.02</v>
+      </c>
+      <c r="E52">
         <v>3</v>
       </c>
-      <c r="C17">
-        <v>703.02</v>
-      </c>
-      <c r="E17">
+      <c r="F52">
         <v>3125.37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update report_mak1g11 with analysis section and add more statistics
</commit_message>
<xml_diff>
--- a/report/stats.xlsx
+++ b/report/stats.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fuzzy Dingo\Documents\COMP6203\AgentElman\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Java\AgentElman\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="38">
   <si>
     <t>Game</t>
   </si>
@@ -121,12 +121,30 @@
   <si>
     <t>Agent Name</t>
   </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +167,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,12 +211,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -246,7 +272,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -388,7 +414,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -530,7 +556,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -672,7 +698,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -814,7 +840,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -956,7 +982,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -1098,11 +1124,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1227,6 +1251,389 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$121</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cortana</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$121:$H$136</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2227.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2090.3200000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2070.5466666699999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2120.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2228.4079999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2427.1333333299999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2371.82857143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2177.21875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2058.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1989.7090000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1805.6509090899999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1981.59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1974.85384615</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1914.1014285700001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2007.7093333299999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2124.8156250000002</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$138</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>westridge</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$138:$I$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$138:$H$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1708.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.495000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-41.723333333299998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.0175000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-195.292</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>419.78166666700002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>765.62142857100002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>929.49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>687.34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>849.12900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1059.48909091</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>883.44749999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1078.99692308</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1139.78285714</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1286.556</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1351.8575000000001</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$155</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AbsMTree</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$155:$I$170</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$155:$H$170</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1551.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-818.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-490.563333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>299.90249999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>551.92200000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>488.99833333300001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>833.89</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>875.40499999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>957.61111111100001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1115.67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1144.9718181799999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1220.6775</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1413.9715384599999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1421.5214285699999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1416.6066666700001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1335.2850000000001</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1235,439 +1642,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="376006160"/>
-        <c:axId val="376003360"/>
+        <c:axId val="157881072"/>
+        <c:axId val="157881632"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="7"/>
-                <c:order val="7"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$121</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Cortana</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$121:$H$136</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="16"/>
-                      <c:pt idx="0">
-                        <c:v>2227.35</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2090.3200000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2070.5466666699999</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>2120.4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>2228.4079999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>2427.1333333299999</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>2371.82857143</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2177.21875</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>2058.4</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1989.7090000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1805.6509090899999</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>1981.59</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>1974.85384615</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>1914.1014285700001</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2007.7093333299999</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>2124.8156250000002</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="8"/>
-                <c:order val="8"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$138</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>westridge</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$I$138:$I$153</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="16"/>
-                      <c:pt idx="0">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>18</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>21</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>25</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>28</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>30</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>34</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>38</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>42</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>43</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$138:$H$153</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="16"/>
-                      <c:pt idx="0">
-                        <c:v>1708.04</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>67.495000000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>-41.723333333299998</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>-4.0175000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>-195.292</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>419.78166666700002</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>765.62142857100002</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>929.49</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>687.34</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>849.12900000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1059.48909091</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>883.44749999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>1078.99692308</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>1139.78285714</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>1286.556</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>1351.8575000000001</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="9"/>
-                <c:order val="9"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$155</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>AbsMTree</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent4">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$I$155:$I$170</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="16"/>
-                      <c:pt idx="0">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>18</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>26</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>27</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>33</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>36</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>37</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>43</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>44</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$155:$H$170</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="16"/>
-                      <c:pt idx="0">
-                        <c:v>1551.27</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>-818.78</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>-490.563333333</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>299.90249999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>551.92200000000003</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>488.99833333300001</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>833.89</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>875.40499999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>957.61111111100001</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1115.67</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1144.9718181799999</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>1220.6775</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>1413.9715384599999</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>1421.5214285699999</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>1416.6066666700001</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>1335.2850000000001</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-              </c15:ser>
-            </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="10"/>
@@ -1675,7 +1653,7 @@
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$172</c15:sqref>
                         </c15:formulaRef>
@@ -1690,7 +1668,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent5">
                         <a:lumMod val="60000"/>
@@ -1706,7 +1684,7 @@
                 <c:xVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$172:$I$187</c15:sqref>
                         </c15:formulaRef>
@@ -1769,7 +1747,7 @@
                 <c:yVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$172:$H$187</c15:sqref>
                         </c15:formulaRef>
@@ -1838,7 +1816,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$189</c15:sqref>
@@ -1854,7 +1832,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent6">
                         <a:lumMod val="60000"/>
@@ -1869,7 +1847,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$189:$I$204</c15:sqref>
@@ -1932,7 +1910,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$189:$H$204</c15:sqref>
@@ -2002,7 +1980,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$206</c15:sqref>
@@ -2018,7 +1996,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent1">
                         <a:lumMod val="80000"/>
@@ -2034,7 +2012,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$206:$I$221</c15:sqref>
@@ -2097,7 +2075,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$206:$H$221</c15:sqref>
@@ -2167,7 +2145,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$223</c15:sqref>
@@ -2183,7 +2161,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent2">
                         <a:lumMod val="80000"/>
@@ -2199,7 +2177,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$223:$I$238</c15:sqref>
@@ -2262,7 +2240,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$223:$H$238</c15:sqref>
@@ -2332,7 +2310,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$240</c15:sqref>
@@ -2348,7 +2326,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent3">
                         <a:lumMod val="80000"/>
@@ -2364,7 +2342,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$240:$I$255</c15:sqref>
@@ -2427,7 +2405,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$240:$H$255</c15:sqref>
@@ -2497,7 +2475,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$257</c15:sqref>
@@ -2513,7 +2491,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent4">
                         <a:lumMod val="80000"/>
@@ -2529,7 +2507,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$257:$I$272</c15:sqref>
@@ -2592,7 +2570,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$257:$H$272</c15:sqref>
@@ -2662,7 +2640,7 @@
                 <c:order val="16"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$274</c15:sqref>
@@ -2678,7 +2656,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent5">
                         <a:lumMod val="80000"/>
@@ -2694,7 +2672,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$274:$I$289</c15:sqref>
@@ -2757,7 +2735,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$274:$H$289</c15:sqref>
@@ -2827,7 +2805,7 @@
                 <c:order val="17"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$291</c15:sqref>
@@ -2843,7 +2821,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent6">
                         <a:lumMod val="80000"/>
@@ -2859,7 +2837,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$291:$I$306</c15:sqref>
@@ -2922,7 +2900,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$291:$H$306</c15:sqref>
@@ -2992,7 +2970,7 @@
                 <c:order val="18"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$308</c15:sqref>
@@ -3008,7 +2986,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent1">
                         <a:lumMod val="80000"/>
@@ -3023,7 +3001,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$308:$I$323</c15:sqref>
@@ -3086,7 +3064,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$308:$H$323</c15:sqref>
@@ -3156,7 +3134,7 @@
                 <c:order val="19"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$325</c15:sqref>
@@ -3172,7 +3150,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent2">
                         <a:lumMod val="80000"/>
@@ -3187,7 +3165,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$325:$I$340</c15:sqref>
@@ -3250,7 +3228,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$325:$H$340</c15:sqref>
@@ -3320,7 +3298,7 @@
                 <c:order val="20"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$342</c15:sqref>
@@ -3336,7 +3314,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent3">
                         <a:lumMod val="80000"/>
@@ -3351,7 +3329,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$342:$I$357</c15:sqref>
@@ -3414,7 +3392,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$342:$H$357</c15:sqref>
@@ -3484,7 +3462,7 @@
                 <c:order val="21"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$359</c15:sqref>
@@ -3500,7 +3478,7 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="19050" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent4">
                         <a:lumMod val="80000"/>
@@ -3515,7 +3493,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$359:$I$374</c15:sqref>
@@ -3578,7 +3556,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$359:$H$374</c15:sqref>
@@ -3646,7 +3624,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="376006160"/>
+        <c:axId val="157881072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3674,9 +3652,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -3703,12 +3681,705 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376003360"/>
+        <c:crossAx val="157881632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376003360"/>
+        <c:axId val="157881632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="157881072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Scores</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> for Agent Elman</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$104:$E$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>3640.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2517.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3108.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3133.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>787.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3029.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3113.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1601.57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-227.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1183.4100000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>611.42999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>674.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2451.2199999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3657</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4475.46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>703.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="785785744"/>
+        <c:axId val="785787424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="785785744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="785787424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="785787424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="785785744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Mean Agent Scores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>3310.2618750000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3099.5756249999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2698.1581249999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2659.6350000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2492.5543750000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2367.6750000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2153.8125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2124.8156250000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1351.8575000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1335.2850000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1250.8143749999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1045.605</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>975.00250000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>869.18187499999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>800.82</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>301.22687500000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>220.16374999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>123.816875</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-345.96</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-611.90750000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-694.87687500000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-2747.183125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="787003840"/>
+        <c:axId val="785429408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="787003840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="785429408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="785429408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3765,7 +4436,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376006160"/>
+        <c:crossAx val="787003840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3777,38 +4448,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3886,7 +4525,1110 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4434,13 +6176,73 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>985836</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Really Colourful">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4700,10 +6502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M375"/>
+  <dimension ref="A1:T375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B142" workbookViewId="0">
-      <selection activeCell="U165" sqref="U165"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4716,7 +6518,7 @@
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -4745,7 +6547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4780,8 +6582,11 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="1">
+        <v>3310.2618750000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4816,8 +6621,11 @@
       <c r="M3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="1">
+        <v>3099.5756249999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4852,8 +6660,11 @@
       <c r="M4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" s="1">
+        <v>2698.1581249999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4888,8 +6699,11 @@
       <c r="M5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" s="1">
+        <v>2659.6350000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4924,8 +6738,11 @@
       <c r="M6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6" s="1">
+        <v>2492.5543750000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -4960,8 +6777,11 @@
       <c r="M7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O7" s="1">
+        <v>2367.6750000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4996,8 +6816,11 @@
       <c r="M8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" s="1">
+        <v>2153.8125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -5032,8 +6855,11 @@
       <c r="M9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9" s="1">
+        <v>2124.8156250000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -5068,8 +6894,11 @@
       <c r="M10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" s="1">
+        <v>1351.8575000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5104,8 +6933,11 @@
       <c r="M11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" s="1">
+        <v>1335.2850000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5140,8 +6972,11 @@
       <c r="M12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" s="1">
+        <v>1250.8143749999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5176,8 +7011,11 @@
       <c r="M13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O13" s="1">
+        <v>1045.605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -5212,8 +7050,11 @@
       <c r="M14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14" s="1">
+        <v>975.00250000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -5248,8 +7089,11 @@
       <c r="M15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O15" s="1">
+        <v>869.18187499999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -5284,8 +7128,11 @@
       <c r="M16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O16" s="1">
+        <v>800.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -5320,8 +7167,11 @@
       <c r="M17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="1">
+        <v>301.22687500000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -5341,8 +7191,11 @@
       <c r="M18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O18" s="1">
+        <v>220.16374999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -5374,8 +7227,11 @@
       <c r="M19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O19" s="1">
+        <v>123.816875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -5407,8 +7263,11 @@
       <c r="M20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" s="1">
+        <v>-345.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -5440,8 +7299,11 @@
       <c r="M21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21" s="1">
+        <v>-611.90750000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -5473,8 +7335,11 @@
       <c r="M22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="1">
+        <v>-694.87687500000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -5506,8 +7371,11 @@
       <c r="M23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23" s="1">
+        <v>-2747.183125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -5540,7 +7408,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -5573,7 +7441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -5606,7 +7474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -5639,7 +7507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -5672,7 +7540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -5705,7 +7573,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -5738,7 +7606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -5771,7 +7639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -8005,7 +9873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>7</v>
       </c>
@@ -8032,7 +9900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>7</v>
       </c>
@@ -8059,7 +9927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>7</v>
       </c>
@@ -8086,7 +9954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>7</v>
       </c>
@@ -8113,7 +9981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>7</v>
       </c>
@@ -8140,7 +10008,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>7</v>
       </c>
@@ -8166,8 +10034,29 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N118" t="s">
+        <v>32</v>
+      </c>
+      <c r="O118" t="s">
+        <v>7</v>
+      </c>
+      <c r="P118" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>7</v>
+      </c>
+      <c r="R118" t="s">
+        <v>11</v>
+      </c>
+      <c r="S118" t="s">
+        <v>7</v>
+      </c>
+      <c r="T118" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>7</v>
       </c>
@@ -8193,8 +10082,32 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="120" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N119" t="s">
+        <v>33</v>
+      </c>
+      <c r="O119">
+        <v>2484.4450000000002</v>
+      </c>
+      <c r="P119">
+        <f>(3203.03+3555.44)/2</f>
+        <v>3379.2350000000001</v>
+      </c>
+      <c r="Q119">
+        <v>2484.4450000000002</v>
+      </c>
+      <c r="R119">
+        <f>(3203.03+3555.44)/2</f>
+        <v>3379.2350000000001</v>
+      </c>
+      <c r="S119">
+        <v>2484.4450000000002</v>
+      </c>
+      <c r="T119">
+        <f>(3203.03+3555.44)/2</f>
+        <v>3379.2350000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
         <v>9</v>
       </c>
@@ -8208,8 +10121,29 @@
         <v>1002.055625</v>
       </c>
       <c r="I120"/>
-    </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N120" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O120" s="3">
+        <v>745.35</v>
+      </c>
+      <c r="P120" s="4">
+        <v>2840.2750000000001</v>
+      </c>
+      <c r="Q120" s="3">
+        <v>745.35</v>
+      </c>
+      <c r="R120" s="4">
+        <v>2840.2750000000001</v>
+      </c>
+      <c r="S120" s="3">
+        <v>745.35</v>
+      </c>
+      <c r="T120" s="4">
+        <v>2840.2750000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>17</v>
       </c>
@@ -8235,8 +10169,29 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N121" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O121">
+        <v>-227.45</v>
+      </c>
+      <c r="P121">
+        <v>1751.04</v>
+      </c>
+      <c r="Q121">
+        <v>-227.45</v>
+      </c>
+      <c r="R121">
+        <v>1751.04</v>
+      </c>
+      <c r="S121">
+        <v>-227.45</v>
+      </c>
+      <c r="T121">
+        <v>1751.04</v>
+      </c>
+    </row>
+    <row r="122" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>17</v>
       </c>
@@ -8262,8 +10217,35 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K122">
+        <v>1751.04</v>
+      </c>
+      <c r="L122">
+        <v>-227.45</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O122">
+        <v>4475.46</v>
+      </c>
+      <c r="P122">
+        <v>4316.2299999999996</v>
+      </c>
+      <c r="Q122">
+        <v>4475.46</v>
+      </c>
+      <c r="R122">
+        <v>4316.2299999999996</v>
+      </c>
+      <c r="S122">
+        <v>4475.46</v>
+      </c>
+      <c r="T122">
+        <v>4316.2299999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>17</v>
       </c>
@@ -8289,8 +10271,35 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K123">
+        <v>2365.87</v>
+      </c>
+      <c r="L123">
+        <v>611.42999999999995</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O123">
+        <v>3123.5349999999999</v>
+      </c>
+      <c r="P123" s="4">
+        <v>3822.09</v>
+      </c>
+      <c r="Q123">
+        <v>3123.5349999999999</v>
+      </c>
+      <c r="R123" s="4">
+        <v>3822.09</v>
+      </c>
+      <c r="S123">
+        <v>3123.5349999999999</v>
+      </c>
+      <c r="T123" s="4">
+        <v>3822.09</v>
+      </c>
+    </row>
+    <row r="124" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>17</v>
       </c>
@@ -8316,8 +10325,14 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K124">
+        <v>2662.66</v>
+      </c>
+      <c r="L124">
+        <v>674.42</v>
+      </c>
+    </row>
+    <row r="125" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>17</v>
       </c>
@@ -8343,8 +10358,14 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K125">
+        <v>2756.96</v>
+      </c>
+      <c r="L125">
+        <v>703.02</v>
+      </c>
+    </row>
+    <row r="126" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>17</v>
       </c>
@@ -8370,8 +10391,14 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K126">
+        <v>2923.59</v>
+      </c>
+      <c r="L126">
+        <v>787.68</v>
+      </c>
+    </row>
+    <row r="127" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>17</v>
       </c>
@@ -8397,8 +10424,14 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K127">
+        <v>2968.19</v>
+      </c>
+      <c r="L127">
+        <v>1183.4100000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>17</v>
       </c>
@@ -8424,8 +10457,14 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K128">
+        <v>3180.74</v>
+      </c>
+      <c r="L128">
+        <v>1601.57</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>17</v>
       </c>
@@ -8451,8 +10490,14 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K129">
+        <v>3203.03</v>
+      </c>
+      <c r="L129">
+        <v>2451.2199999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>17</v>
       </c>
@@ -8478,8 +10523,14 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K130">
+        <v>3555.44</v>
+      </c>
+      <c r="L130">
+        <v>2517.67</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>17</v>
       </c>
@@ -8505,8 +10556,14 @@
         <f t="shared" ref="I131:I194" si="2">D131-612</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K131">
+        <v>3670.28</v>
+      </c>
+      <c r="L131">
+        <v>3029.65</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>17</v>
       </c>
@@ -8532,8 +10589,14 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K132">
+        <v>3777.68</v>
+      </c>
+      <c r="L132">
+        <v>3108.83</v>
+      </c>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>17</v>
       </c>
@@ -8559,8 +10622,14 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K133">
+        <v>3815.79</v>
+      </c>
+      <c r="L133">
+        <v>3113.59</v>
+      </c>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>17</v>
       </c>
@@ -8586,8 +10655,14 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K134">
+        <v>3828.39</v>
+      </c>
+      <c r="L134">
+        <v>3133.48</v>
+      </c>
+    </row>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>17</v>
       </c>
@@ -8613,8 +10688,14 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K135">
+        <v>4037.86</v>
+      </c>
+      <c r="L135">
+        <v>3640.02</v>
+      </c>
+    </row>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>17</v>
       </c>
@@ -8640,8 +10721,14 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="137" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K136">
+        <v>4150.4399999999996</v>
+      </c>
+      <c r="L136">
+        <v>3657</v>
+      </c>
+    </row>
+    <row r="137" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>9</v>
       </c>
@@ -8655,8 +10742,14 @@
         <v>1226.34375</v>
       </c>
       <c r="I137"/>
-    </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K137">
+        <v>4316.2299999999996</v>
+      </c>
+      <c r="L137">
+        <v>4475.46</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>8</v>
       </c>
@@ -8683,7 +10776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>8</v>
       </c>
@@ -8710,7 +10803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>8</v>
       </c>
@@ -8737,7 +10830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>8</v>
       </c>
@@ -8764,7 +10857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>8</v>
       </c>
@@ -8791,7 +10884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>8</v>
       </c>
@@ -8818,7 +10911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>8</v>
       </c>
@@ -14914,6 +17007,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="K122:K137">
+    <sortCondition ref="K122"/>
+  </sortState>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Improved report and added more stats. Report mostly final, maybe needs one more section of analysis
</commit_message>
<xml_diff>
--- a/report/stats.xlsx
+++ b/report/stats.xlsx
@@ -1642,8 +1642,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="157881072"/>
-        <c:axId val="157881632"/>
+        <c:axId val="169960624"/>
+        <c:axId val="169961184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3624,7 +3624,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157881072"/>
+        <c:axId val="169960624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,12 +3681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157881632"/>
+        <c:crossAx val="169961184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157881632"/>
+        <c:axId val="169961184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3743,7 +3743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157881072"/>
+        <c:crossAx val="169960624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3757,7 +3757,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3869,7 +3868,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3987,11 +3985,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="785785744"/>
-        <c:axId val="785787424"/>
+        <c:axId val="169963984"/>
+        <c:axId val="171048496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="785785744"/>
+        <c:axId val="169963984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4034,7 +4032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="785787424"/>
+        <c:crossAx val="171048496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4042,7 +4040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="785787424"/>
+        <c:axId val="171048496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4093,7 +4091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="785785744"/>
+        <c:crossAx val="169963984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4347,11 +4345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="787003840"/>
-        <c:axId val="785429408"/>
+        <c:axId val="171051296"/>
+        <c:axId val="171051856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="787003840"/>
+        <c:axId val="171051296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4374,12 +4372,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="785429408"/>
+        <c:crossAx val="171051856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="785429408"/>
+        <c:axId val="171051856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4436,9 +4434,342 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="787003840"/>
+        <c:crossAx val="171051296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$X$7:$X$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$7:$W$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="678448608"/>
+        <c:axId val="678448048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="678448608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678448048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="678448048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678448608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4566,6 +4897,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6144,6 +6515,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6231,6 +7118,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6502,10 +7419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T375"/>
+  <dimension ref="A1:X375"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6518,7 +7435,7 @@
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -6547,7 +7464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6586,7 +7503,7 @@
         <v>3310.2618750000001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6625,7 +7542,7 @@
         <v>3099.5756249999999</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -6664,7 +7581,7 @@
         <v>2698.1581249999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6703,7 +7620,7 @@
         <v>2659.6350000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6742,7 +7659,7 @@
         <v>2492.5543750000002</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -6780,8 +7697,14 @@
       <c r="O7" s="1">
         <v>2367.6750000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <v>130</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6819,8 +7742,14 @@
       <c r="O8" s="1">
         <v>2153.8125</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <v>130</v>
+      </c>
+      <c r="X8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -6858,8 +7787,14 @@
       <c r="O9" s="1">
         <v>2124.8156250000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <v>130</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6897,8 +7832,14 @@
       <c r="O10" s="1">
         <v>1351.8575000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W10">
+        <v>130</v>
+      </c>
+      <c r="X10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -6936,8 +7877,14 @@
       <c r="O11" s="1">
         <v>1335.2850000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <v>129</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6975,8 +7922,14 @@
       <c r="O12" s="1">
         <v>1250.8143749999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W12">
+        <v>128</v>
+      </c>
+      <c r="X12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -7014,8 +7967,14 @@
       <c r="O13" s="1">
         <v>1045.605</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W13">
+        <v>127</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7053,8 +8012,14 @@
       <c r="O14" s="1">
         <v>975.00250000000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W14">
+        <v>125</v>
+      </c>
+      <c r="X14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -7092,8 +8057,14 @@
       <c r="O15" s="1">
         <v>869.18187499999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W15">
+        <v>122</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -7131,8 +8102,14 @@
       <c r="O16" s="1">
         <v>800.82</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W16">
+        <v>119</v>
+      </c>
+      <c r="X16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -7170,8 +8147,14 @@
       <c r="O17" s="1">
         <v>301.22687500000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W17">
+        <v>115</v>
+      </c>
+      <c r="X17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -7194,8 +8177,14 @@
       <c r="O18" s="1">
         <v>220.16374999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W18" s="1">
+        <v>111</v>
+      </c>
+      <c r="X18" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -7230,8 +8219,14 @@
       <c r="O19" s="1">
         <v>123.816875</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W19">
+        <v>105</v>
+      </c>
+      <c r="X19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -7266,8 +8261,14 @@
       <c r="O20" s="1">
         <v>-345.96</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W20">
+        <v>98</v>
+      </c>
+      <c r="X20">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -7302,8 +8303,14 @@
       <c r="O21" s="1">
         <v>-611.90750000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W21">
+        <v>90</v>
+      </c>
+      <c r="X21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -7338,8 +8345,14 @@
       <c r="O22" s="1">
         <v>-694.87687500000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W22">
+        <v>81</v>
+      </c>
+      <c r="X22">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -7374,8 +8387,14 @@
       <c r="O23" s="1">
         <v>-2747.183125</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W23">
+        <v>81</v>
+      </c>
+      <c r="X23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -7407,8 +8426,14 @@
       <c r="M24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W24">
+        <v>81</v>
+      </c>
+      <c r="X24">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -7440,8 +8465,14 @@
       <c r="M25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W25">
+        <v>81</v>
+      </c>
+      <c r="X25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -7474,7 +8505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -7507,7 +8538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -7540,7 +8571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -7573,7 +8604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -7606,7 +8637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -7639,7 +8670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>

</xml_diff>